<commit_message>
[MS-VERSS]: Fix watchman warnings
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-VERSS/MS-VERSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-VERSS/MS-VERSS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SHAREPOINT\MS-VERSS\update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-VERSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1867,7 +1867,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1877,7 +1877,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1889,7 +1889,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1899,7 +1899,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1911,7 +1911,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1921,7 +1921,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2043,7 +2043,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2055,7 +2055,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2065,7 +2065,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2077,7 +2077,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2087,7 +2087,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2099,7 +2099,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2109,7 +2109,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2120,7 +2120,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3183,12 +3183,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-VERSS_R17802021.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-VERSS_R17802011.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Verified by derived requirement: MS-VERSS_R17802011.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-VERSS_R17802021.</t>
   </si>
 </sst>
 </file>
@@ -3196,15 +3194,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="yyyy\!\-mm\!\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\!\-mm\!\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3225,7 +3223,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3233,13 +3231,13 @@
       <b/>
       <sz val="16"/>
       <color theme="3" tint="0.39997558519241921"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3252,7 +3250,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3437,7 +3435,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3467,12 +3465,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3503,7 +3501,31 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3539,30 +3561,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5000,7 +4998,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -5014,7 +5012,7 @@
     <col min="10" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>573</v>
       </c>
@@ -5023,7 +5021,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>846</v>
       </c>
@@ -5036,7 +5034,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="B3" s="7" t="s">
         <v>538</v>
       </c>
@@ -5053,130 +5051,130 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="57" t="s">
+    <row r="4" spans="1:10" ht="20.25">
+      <c r="A4" s="45" t="s">
         <v>539</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="26"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="47" t="s">
         <v>560</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="46" t="s">
         <v>561</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="26"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="46" t="s">
         <v>540</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="78" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="35.25" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="50" t="s">
         <v>563</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>564</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10">
       <c r="A12" s="30" t="s">
         <v>9</v>
       </c>
@@ -5186,15 +5184,15 @@
       <c r="C12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="26.25" customHeight="1">
       <c r="A13" s="31" t="s">
         <v>7</v>
       </c>
@@ -5204,15 +5202,15 @@
       <c r="C13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="26"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10">
       <c r="A14" s="32" t="s">
         <v>8</v>
       </c>
@@ -5222,15 +5220,15 @@
       <c r="C14" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="26"/>
     </row>
-    <row r="15" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10">
       <c r="A15" s="33" t="s">
         <v>4</v>
       </c>
@@ -5240,64 +5238,64 @@
       <c r="C15" s="15" t="s">
         <v>567</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
       <c r="J15" s="26"/>
     </row>
-    <row r="16" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="36.75" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="57" t="s">
         <v>569</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="1:12" ht="95.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="95.25" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>570</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
       <c r="J17" s="26"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>568</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="26"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -5326,7 +5324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A20" s="11" t="s">
         <v>26</v>
       </c>
@@ -5351,7 +5349,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
@@ -5376,7 +5374,7 @@
       </c>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A22" s="11" t="s">
         <v>29</v>
       </c>
@@ -5401,7 +5399,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
@@ -5426,7 +5424,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="12" customFormat="1">
       <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
@@ -5451,7 +5449,7 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A25" s="11" t="s">
         <v>34</v>
       </c>
@@ -5478,7 +5476,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="12" customFormat="1" ht="45">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
@@ -5507,7 +5505,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A27" s="11" t="s">
         <v>38</v>
       </c>
@@ -5532,7 +5530,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="12" customFormat="1">
       <c r="A28" s="11" t="s">
         <v>353</v>
       </c>
@@ -5559,7 +5557,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="12" customFormat="1">
       <c r="A29" s="11" t="s">
         <v>354</v>
       </c>
@@ -5586,7 +5584,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A30" s="11" t="s">
         <v>39</v>
       </c>
@@ -5611,7 +5609,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="12" customFormat="1" ht="30">
       <c r="A31" s="11" t="s">
         <v>340</v>
       </c>
@@ -5638,7 +5636,7 @@
       </c>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="12" customFormat="1">
       <c r="A32" s="11" t="s">
         <v>341</v>
       </c>
@@ -5665,7 +5663,7 @@
       </c>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="12" customFormat="1">
       <c r="A33" s="11" t="s">
         <v>350</v>
       </c>
@@ -5692,7 +5690,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" s="12" customFormat="1">
       <c r="A34" s="11" t="s">
         <v>40</v>
       </c>
@@ -5717,7 +5715,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A35" s="11" t="s">
         <v>43</v>
       </c>
@@ -5742,7 +5740,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A36" s="11" t="s">
         <v>44</v>
       </c>
@@ -5767,7 +5765,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A37" s="11" t="s">
         <v>47</v>
       </c>
@@ -5792,7 +5790,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" s="12" customFormat="1">
       <c r="A38" s="11" t="s">
         <v>48</v>
       </c>
@@ -5817,7 +5815,7 @@
       </c>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" s="12" customFormat="1">
       <c r="A39" s="11" t="s">
         <v>50</v>
       </c>
@@ -5842,7 +5840,7 @@
       </c>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A40" s="11" t="s">
         <v>52</v>
       </c>
@@ -5867,7 +5865,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A41" s="11" t="s">
         <v>54</v>
       </c>
@@ -5892,7 +5890,7 @@
       </c>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A42" s="11" t="s">
         <v>56</v>
       </c>
@@ -5917,7 +5915,7 @@
       </c>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A43" s="11" t="s">
         <v>58</v>
       </c>
@@ -5942,7 +5940,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" s="12" customFormat="1">
       <c r="A44" s="11" t="s">
         <v>60</v>
       </c>
@@ -5967,7 +5965,7 @@
       </c>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" s="12" customFormat="1">
       <c r="A45" s="11" t="s">
         <v>62</v>
       </c>
@@ -5992,7 +5990,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A46" s="11" t="s">
         <v>64</v>
       </c>
@@ -6017,7 +6015,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" s="12" customFormat="1">
       <c r="A47" s="11" t="s">
         <v>66</v>
       </c>
@@ -6042,7 +6040,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" s="12" customFormat="1">
       <c r="A48" s="11" t="s">
         <v>68</v>
       </c>
@@ -6067,7 +6065,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A49" s="11" t="s">
         <v>71</v>
       </c>
@@ -6092,7 +6090,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A50" s="11" t="s">
         <v>73</v>
       </c>
@@ -6117,7 +6115,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" s="12" customFormat="1">
       <c r="A51" s="11" t="s">
         <v>74</v>
       </c>
@@ -6142,7 +6140,7 @@
       </c>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" s="12" customFormat="1">
       <c r="A52" s="11" t="s">
         <v>76</v>
       </c>
@@ -6167,7 +6165,7 @@
       </c>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" s="12" customFormat="1">
       <c r="A53" s="11" t="s">
         <v>78</v>
       </c>
@@ -6192,7 +6190,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A54" s="11" t="s">
         <v>85</v>
       </c>
@@ -6217,7 +6215,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A55" s="11" t="s">
         <v>81</v>
       </c>
@@ -6242,7 +6240,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" s="12" customFormat="1">
       <c r="A56" s="11" t="s">
         <v>82</v>
       </c>
@@ -6267,7 +6265,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A57" s="11" t="s">
         <v>84</v>
       </c>
@@ -6292,7 +6290,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" s="12" customFormat="1">
       <c r="A58" s="11" t="s">
         <v>86</v>
       </c>
@@ -6317,7 +6315,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A59" s="11" t="s">
         <v>668</v>
       </c>
@@ -6342,7 +6340,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A60" s="11" t="s">
         <v>89</v>
       </c>
@@ -6367,7 +6365,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A61" s="11" t="s">
         <v>90</v>
       </c>
@@ -6392,7 +6390,7 @@
       </c>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A62" s="11" t="s">
         <v>92</v>
       </c>
@@ -6417,7 +6415,7 @@
       </c>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A63" s="11" t="s">
         <v>93</v>
       </c>
@@ -6442,7 +6440,7 @@
       </c>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" s="12" customFormat="1">
       <c r="A64" s="11" t="s">
         <v>94</v>
       </c>
@@ -6467,7 +6465,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A65" s="11" t="s">
         <v>95</v>
       </c>
@@ -6492,7 +6490,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A66" s="11" t="s">
         <v>97</v>
       </c>
@@ -6517,7 +6515,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" s="12" customFormat="1" ht="310.5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9" s="12" customFormat="1" ht="330">
       <c r="A67" s="11" t="s">
         <v>98</v>
       </c>
@@ -6542,7 +6540,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9" s="12" customFormat="1">
       <c r="A68" s="11" t="s">
         <v>99</v>
       </c>
@@ -6567,7 +6565,7 @@
       </c>
       <c r="I68" s="19"/>
     </row>
-    <row r="69" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9" s="12" customFormat="1">
       <c r="A69" s="11" t="s">
         <v>100</v>
       </c>
@@ -6592,7 +6590,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9" s="12" customFormat="1">
       <c r="A70" s="11" t="s">
         <v>102</v>
       </c>
@@ -6617,7 +6615,7 @@
       </c>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9" s="12" customFormat="1">
       <c r="A71" s="11" t="s">
         <v>104</v>
       </c>
@@ -6642,7 +6640,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9" s="12" customFormat="1">
       <c r="A72" s="11" t="s">
         <v>105</v>
       </c>
@@ -6667,7 +6665,7 @@
       </c>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9" s="12" customFormat="1">
       <c r="A73" s="11" t="s">
         <v>107</v>
       </c>
@@ -6692,7 +6690,7 @@
       </c>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9" s="12" customFormat="1">
       <c r="A74" s="11" t="s">
         <v>109</v>
       </c>
@@ -6717,7 +6715,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:9" s="12" customFormat="1">
       <c r="A75" s="11" t="s">
         <v>110</v>
       </c>
@@ -6742,7 +6740,7 @@
       </c>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A76" s="11" t="s">
         <v>112</v>
       </c>
@@ -6767,7 +6765,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9" s="12" customFormat="1">
       <c r="A77" s="11" t="s">
         <v>113</v>
       </c>
@@ -6792,7 +6790,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9" s="12" customFormat="1">
       <c r="A78" s="11" t="s">
         <v>115</v>
       </c>
@@ -6817,7 +6815,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9" s="12" customFormat="1">
       <c r="A79" s="11" t="s">
         <v>117</v>
       </c>
@@ -6842,7 +6840,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" s="12" customFormat="1" ht="148.5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9" s="12" customFormat="1" ht="150">
       <c r="A80" s="11" t="s">
         <v>119</v>
       </c>
@@ -6867,7 +6865,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" s="12" customFormat="1">
       <c r="A81" s="11" t="s">
         <v>120</v>
       </c>
@@ -6892,7 +6890,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:9" s="12" customFormat="1">
       <c r="A82" s="11" t="s">
         <v>122</v>
       </c>
@@ -6917,7 +6915,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" s="12" customFormat="1" ht="162" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:9" s="12" customFormat="1" ht="165">
       <c r="A83" s="11" t="s">
         <v>125</v>
       </c>
@@ -6942,7 +6940,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9" s="12" customFormat="1">
       <c r="A84" s="11" t="s">
         <v>126</v>
       </c>
@@ -6967,7 +6965,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:9" s="12" customFormat="1">
       <c r="A85" s="11" t="s">
         <v>127</v>
       </c>
@@ -6992,7 +6990,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:9" s="12" customFormat="1">
       <c r="A86" s="11" t="s">
         <v>129</v>
       </c>
@@ -7017,7 +7015,7 @@
       </c>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A87" s="11" t="s">
         <v>130</v>
       </c>
@@ -7042,7 +7040,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A88" s="11" t="s">
         <v>669</v>
       </c>
@@ -7069,7 +7067,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:9" s="12" customFormat="1">
       <c r="A89" s="11" t="s">
         <v>131</v>
       </c>
@@ -7094,7 +7092,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A90" s="11" t="s">
         <v>132</v>
       </c>
@@ -7119,7 +7117,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A91" s="11" t="s">
         <v>134</v>
       </c>
@@ -7146,7 +7144,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:9" s="12" customFormat="1">
       <c r="A92" s="11" t="s">
         <v>135</v>
       </c>
@@ -7171,7 +7169,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:9" s="12" customFormat="1">
       <c r="A93" s="11" t="s">
         <v>136</v>
       </c>
@@ -7196,7 +7194,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:9" s="12" customFormat="1">
       <c r="A94" s="11" t="s">
         <v>137</v>
       </c>
@@ -7221,7 +7219,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A95" s="11" t="s">
         <v>138</v>
       </c>
@@ -7246,7 +7244,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:9" s="12" customFormat="1">
       <c r="A96" s="11" t="s">
         <v>139</v>
       </c>
@@ -7271,7 +7269,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:9" s="12" customFormat="1">
       <c r="A97" s="11" t="s">
         <v>141</v>
       </c>
@@ -7296,7 +7294,7 @@
       </c>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:9" s="12" customFormat="1">
       <c r="A98" s="11" t="s">
         <v>143</v>
       </c>
@@ -7321,7 +7319,7 @@
       </c>
       <c r="I98" s="17"/>
     </row>
-    <row r="99" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A99" s="11" t="s">
         <v>145</v>
       </c>
@@ -7346,7 +7344,7 @@
       </c>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:9" s="12" customFormat="1">
       <c r="A100" s="11" t="s">
         <v>147</v>
       </c>
@@ -7371,7 +7369,7 @@
       </c>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:9" s="12" customFormat="1">
       <c r="A101" s="11" t="s">
         <v>150</v>
       </c>
@@ -7396,7 +7394,7 @@
       </c>
       <c r="I101" s="17"/>
     </row>
-    <row r="102" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A102" s="11" t="s">
         <v>152</v>
       </c>
@@ -7421,7 +7419,7 @@
       </c>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A103" s="11" t="s">
         <v>153</v>
       </c>
@@ -7446,7 +7444,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A104" s="11" t="s">
         <v>155</v>
       </c>
@@ -7471,7 +7469,7 @@
       </c>
       <c r="I104" s="17"/>
     </row>
-    <row r="105" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A105" s="11" t="s">
         <v>157</v>
       </c>
@@ -7496,7 +7494,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A106" s="11" t="s">
         <v>158</v>
       </c>
@@ -7521,7 +7519,7 @@
       </c>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A107" s="11" t="s">
         <v>160</v>
       </c>
@@ -7546,7 +7544,7 @@
       </c>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A108" s="11" t="s">
         <v>162</v>
       </c>
@@ -7571,7 +7569,7 @@
       </c>
       <c r="I108" s="19"/>
     </row>
-    <row r="109" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A109" s="11" t="s">
         <v>164</v>
       </c>
@@ -7596,7 +7594,7 @@
       </c>
       <c r="I109" s="19"/>
     </row>
-    <row r="110" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A110" s="11" t="s">
         <v>166</v>
       </c>
@@ -7621,7 +7619,7 @@
       </c>
       <c r="I110" s="19"/>
     </row>
-    <row r="111" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A111" s="11" t="s">
         <v>168</v>
       </c>
@@ -7646,7 +7644,7 @@
       </c>
       <c r="I111" s="19"/>
     </row>
-    <row r="112" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A112" s="11" t="s">
         <v>171</v>
       </c>
@@ -7671,7 +7669,7 @@
       </c>
       <c r="I112" s="19"/>
     </row>
-    <row r="113" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A113" s="11" t="s">
         <v>173</v>
       </c>
@@ -7696,7 +7694,7 @@
       </c>
       <c r="I113" s="19"/>
     </row>
-    <row r="114" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A114" s="11" t="s">
         <v>174</v>
       </c>
@@ -7721,7 +7719,7 @@
       </c>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A115" s="11" t="s">
         <v>175</v>
       </c>
@@ -7746,7 +7744,7 @@
       </c>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A116" s="11" t="s">
         <v>177</v>
       </c>
@@ -7771,7 +7769,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A117" s="11" t="s">
         <v>179</v>
       </c>
@@ -7796,7 +7794,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A118" s="11" t="s">
         <v>181</v>
       </c>
@@ -7821,7 +7819,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A119" s="11" t="s">
         <v>183</v>
       </c>
@@ -7846,7 +7844,7 @@
       </c>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A120" s="11" t="s">
         <v>185</v>
       </c>
@@ -7871,7 +7869,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A121" s="11" t="s">
         <v>187</v>
       </c>
@@ -7896,7 +7894,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A122" s="11" t="s">
         <v>188</v>
       </c>
@@ -7921,7 +7919,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:9" s="12" customFormat="1">
       <c r="A123" s="11" t="s">
         <v>189</v>
       </c>
@@ -7946,7 +7944,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A124" s="11" t="s">
         <v>191</v>
       </c>
@@ -7971,7 +7969,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A125" s="11" t="s">
         <v>192</v>
       </c>
@@ -7996,7 +7994,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:9" s="12" customFormat="1">
       <c r="A126" s="11" t="s">
         <v>374</v>
       </c>
@@ -8021,7 +8019,7 @@
       </c>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A127" s="11" t="s">
         <v>375</v>
       </c>
@@ -8046,7 +8044,7 @@
       </c>
       <c r="I127" s="17"/>
     </row>
-    <row r="128" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A128" s="11" t="s">
         <v>194</v>
       </c>
@@ -8071,7 +8069,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A129" s="11" t="s">
         <v>197</v>
       </c>
@@ -8096,7 +8094,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:9" s="12" customFormat="1">
       <c r="A130" s="11" t="s">
         <v>198</v>
       </c>
@@ -8121,7 +8119,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A131" s="11" t="s">
         <v>199</v>
       </c>
@@ -8146,7 +8144,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:9" s="12" customFormat="1">
       <c r="A132" s="11" t="s">
         <v>201</v>
       </c>
@@ -8171,7 +8169,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A133" s="11" t="s">
         <v>202</v>
       </c>
@@ -8196,7 +8194,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:9" s="12" customFormat="1">
       <c r="A134" s="11" t="s">
         <v>859</v>
       </c>
@@ -8221,7 +8219,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:9" s="12" customFormat="1">
       <c r="A135" s="11" t="s">
         <v>860</v>
       </c>
@@ -8246,7 +8244,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A136" s="11" t="s">
         <v>863</v>
       </c>
@@ -8271,7 +8269,7 @@
       </c>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" s="12" customFormat="1" ht="108" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:9" s="12" customFormat="1" ht="120">
       <c r="A137" s="11" t="s">
         <v>204</v>
       </c>
@@ -8296,7 +8294,7 @@
       </c>
       <c r="I137" s="17"/>
     </row>
-    <row r="138" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:9" s="12" customFormat="1">
       <c r="A138" s="11" t="s">
         <v>206</v>
       </c>
@@ -8321,7 +8319,7 @@
       </c>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A139" s="11" t="s">
         <v>865</v>
       </c>
@@ -8346,7 +8344,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" s="12" customFormat="1" ht="216" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:9" s="12" customFormat="1" ht="210">
       <c r="A140" s="11" t="s">
         <v>207</v>
       </c>
@@ -8371,7 +8369,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A141" s="11" t="s">
         <v>209</v>
       </c>
@@ -8396,7 +8394,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A142" s="11" t="s">
         <v>589</v>
       </c>
@@ -8421,7 +8419,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A143" s="11" t="s">
         <v>581</v>
       </c>
@@ -8448,7 +8446,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="144" spans="1:9" s="12" customFormat="1" ht="175.5" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:9" s="12" customFormat="1" ht="180">
       <c r="A144" s="11" t="s">
         <v>210</v>
       </c>
@@ -8475,7 +8473,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A145" s="11" t="s">
         <v>416</v>
       </c>
@@ -8500,7 +8498,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:9" s="12" customFormat="1">
       <c r="A146" s="11" t="s">
         <v>213</v>
       </c>
@@ -8525,7 +8523,7 @@
       </c>
       <c r="I146" s="19"/>
     </row>
-    <row r="147" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:9" s="12" customFormat="1">
       <c r="A147" s="11" t="s">
         <v>215</v>
       </c>
@@ -8550,7 +8548,7 @@
       </c>
       <c r="I147" s="19"/>
     </row>
-    <row r="148" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A148" s="11" t="s">
         <v>216</v>
       </c>
@@ -8575,7 +8573,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A149" s="11" t="s">
         <v>217</v>
       </c>
@@ -8600,7 +8598,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A150" s="11" t="s">
         <v>218</v>
       </c>
@@ -8625,7 +8623,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:9" s="12" customFormat="1">
       <c r="A151" s="11" t="s">
         <v>219</v>
       </c>
@@ -8650,7 +8648,7 @@
       </c>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A152" s="11" t="s">
         <v>221</v>
       </c>
@@ -8675,7 +8673,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A153" s="11" t="s">
         <v>222</v>
       </c>
@@ -8700,7 +8698,7 @@
       </c>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:9" s="12" customFormat="1">
       <c r="A154" s="11" t="s">
         <v>389</v>
       </c>
@@ -8725,7 +8723,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:9" s="12" customFormat="1">
       <c r="A155" s="11" t="s">
         <v>390</v>
       </c>
@@ -8750,7 +8748,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A156" s="11" t="s">
         <v>224</v>
       </c>
@@ -8775,7 +8773,7 @@
       </c>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A157" s="11" t="s">
         <v>227</v>
       </c>
@@ -8800,7 +8798,7 @@
       </c>
       <c r="I157" s="17"/>
     </row>
-    <row r="158" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:9" s="12" customFormat="1">
       <c r="A158" s="11" t="s">
         <v>228</v>
       </c>
@@ -8825,7 +8823,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A159" s="11" t="s">
         <v>230</v>
       </c>
@@ -8850,7 +8848,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:9" s="12" customFormat="1">
       <c r="A160" s="11" t="s">
         <v>233</v>
       </c>
@@ -8875,7 +8873,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A161" s="11" t="s">
         <v>235</v>
       </c>
@@ -8900,7 +8898,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:9" s="12" customFormat="1">
       <c r="A162" s="11" t="s">
         <v>867</v>
       </c>
@@ -8925,7 +8923,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:9" s="12" customFormat="1">
       <c r="A163" s="11" t="s">
         <v>868</v>
       </c>
@@ -8950,7 +8948,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:9" s="12" customFormat="1">
       <c r="A164" s="11" t="s">
         <v>871</v>
       </c>
@@ -8975,7 +8973,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" s="12" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:9" s="12" customFormat="1" ht="135">
       <c r="A165" s="11" t="s">
         <v>237</v>
       </c>
@@ -9000,7 +8998,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:9" s="12" customFormat="1">
       <c r="A166" s="11" t="s">
         <v>239</v>
       </c>
@@ -9025,7 +9023,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:9" s="12" customFormat="1">
       <c r="A167" s="11" t="s">
         <v>240</v>
       </c>
@@ -9050,7 +9048,7 @@
       </c>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A168" s="11" t="s">
         <v>873</v>
       </c>
@@ -9075,7 +9073,7 @@
       </c>
       <c r="I168" s="17"/>
     </row>
-    <row r="169" spans="1:9" s="12" customFormat="1" ht="216" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:9" s="12" customFormat="1" ht="210">
       <c r="A169" s="11" t="s">
         <v>241</v>
       </c>
@@ -9100,7 +9098,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A170" s="11" t="s">
         <v>243</v>
       </c>
@@ -9125,7 +9123,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A171" s="11" t="s">
         <v>244</v>
       </c>
@@ -9150,7 +9148,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A172" s="11" t="s">
         <v>391</v>
       </c>
@@ -9175,7 +9173,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" s="12" customFormat="1" ht="175.5" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:9" s="12" customFormat="1" ht="165">
       <c r="A173" s="11" t="s">
         <v>245</v>
       </c>
@@ -9202,7 +9200,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="174" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:9" s="12" customFormat="1">
       <c r="A174" s="11" t="s">
         <v>247</v>
       </c>
@@ -9227,7 +9225,7 @@
       </c>
       <c r="I174" s="19"/>
     </row>
-    <row r="175" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:9" s="12" customFormat="1">
       <c r="A175" s="11" t="s">
         <v>249</v>
       </c>
@@ -9252,7 +9250,7 @@
       </c>
       <c r="I175" s="19"/>
     </row>
-    <row r="176" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A176" s="11" t="s">
         <v>251</v>
       </c>
@@ -9279,7 +9277,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="177" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A177" s="11" t="s">
         <v>252</v>
       </c>
@@ -9303,10 +9301,10 @@
         <v>18</v>
       </c>
       <c r="I177" s="19" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A178" s="11" t="s">
         <v>253</v>
       </c>
@@ -9330,10 +9328,10 @@
         <v>18</v>
       </c>
       <c r="I178" s="19" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A179" s="11" t="s">
         <v>254</v>
       </c>
@@ -9358,7 +9356,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A180" s="11" t="s">
         <v>256</v>
       </c>
@@ -9383,7 +9381,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:9" s="12" customFormat="1">
       <c r="A181" s="11" t="s">
         <v>257</v>
       </c>
@@ -9408,7 +9406,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A182" s="11" t="s">
         <v>259</v>
       </c>
@@ -9433,7 +9431,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A183" s="11" t="s">
         <v>260</v>
       </c>
@@ -9458,7 +9456,7 @@
       </c>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A184" s="11" t="s">
         <v>393</v>
       </c>
@@ -9483,7 +9481,7 @@
       </c>
       <c r="I184" s="19"/>
     </row>
-    <row r="185" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A185" s="11" t="s">
         <v>394</v>
       </c>
@@ -9508,7 +9506,7 @@
       </c>
       <c r="I185" s="19"/>
     </row>
-    <row r="186" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A186" s="11" t="s">
         <v>262</v>
       </c>
@@ -9533,7 +9531,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A187" s="11" t="s">
         <v>265</v>
       </c>
@@ -9558,7 +9556,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:9" s="12" customFormat="1">
       <c r="A188" s="11" t="s">
         <v>266</v>
       </c>
@@ -9583,7 +9581,7 @@
       </c>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A189" s="11" t="s">
         <v>268</v>
       </c>
@@ -9608,7 +9606,7 @@
       </c>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:9" s="12" customFormat="1">
       <c r="A190" s="11" t="s">
         <v>271</v>
       </c>
@@ -9633,7 +9631,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A191" s="11" t="s">
         <v>273</v>
       </c>
@@ -9658,7 +9656,7 @@
       </c>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:9" s="12" customFormat="1">
       <c r="A192" s="11" t="s">
         <v>877</v>
       </c>
@@ -9683,7 +9681,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:9" s="12" customFormat="1">
       <c r="A193" s="11" t="s">
         <v>878</v>
       </c>
@@ -9708,7 +9706,7 @@
       </c>
       <c r="I193" s="17"/>
     </row>
-    <row r="194" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:9" s="12" customFormat="1">
       <c r="A194" s="11" t="s">
         <v>881</v>
       </c>
@@ -9733,7 +9731,7 @@
       </c>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" s="12" customFormat="1" ht="108" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:9" s="12" customFormat="1" ht="120">
       <c r="A195" s="11" t="s">
         <v>275</v>
       </c>
@@ -9758,7 +9756,7 @@
       </c>
       <c r="I195" s="17"/>
     </row>
-    <row r="196" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:9" s="12" customFormat="1">
       <c r="A196" s="11" t="s">
         <v>277</v>
       </c>
@@ -9783,7 +9781,7 @@
       </c>
       <c r="I196" s="17"/>
     </row>
-    <row r="197" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A197" s="11" t="s">
         <v>883</v>
       </c>
@@ -9808,7 +9806,7 @@
       </c>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" s="12" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:9" s="12" customFormat="1" ht="210">
       <c r="A198" s="11" t="s">
         <v>278</v>
       </c>
@@ -9833,7 +9831,7 @@
       </c>
       <c r="I198" s="17"/>
     </row>
-    <row r="199" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A199" s="11" t="s">
         <v>280</v>
       </c>
@@ -9858,7 +9856,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A200" s="11" t="s">
         <v>281</v>
       </c>
@@ -9883,7 +9881,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:9" s="12" customFormat="1">
       <c r="A201" s="11" t="s">
         <v>282</v>
       </c>
@@ -9908,7 +9906,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A202" s="11" t="s">
         <v>533</v>
       </c>
@@ -9933,7 +9931,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:9" s="12" customFormat="1">
       <c r="A203" s="11" t="s">
         <v>283</v>
       </c>
@@ -9958,7 +9956,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A204" s="11" t="s">
         <v>285</v>
       </c>
@@ -9983,7 +9981,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A205" s="11" t="s">
         <v>516</v>
       </c>
@@ -10008,7 +10006,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:9" s="12" customFormat="1">
       <c r="A206" s="11" t="s">
         <v>286</v>
       </c>
@@ -10033,7 +10031,7 @@
       </c>
       <c r="I206" s="19"/>
     </row>
-    <row r="207" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:9" s="12" customFormat="1">
       <c r="A207" s="11" t="s">
         <v>287</v>
       </c>
@@ -10058,7 +10056,7 @@
       </c>
       <c r="I207" s="19"/>
     </row>
-    <row r="208" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A208" s="11" t="s">
         <v>289</v>
       </c>
@@ -10083,7 +10081,7 @@
       </c>
       <c r="I208" s="17"/>
     </row>
-    <row r="209" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A209" s="11" t="s">
         <v>290</v>
       </c>
@@ -10108,7 +10106,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:9" s="12" customFormat="1" ht="60">
       <c r="A210" s="11" t="s">
         <v>291</v>
       </c>
@@ -10133,7 +10131,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A211" s="11" t="s">
         <v>292</v>
       </c>
@@ -10158,7 +10156,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A212" s="11" t="s">
         <v>293</v>
       </c>
@@ -10183,7 +10181,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A213" s="11" t="s">
         <v>294</v>
       </c>
@@ -10208,7 +10206,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:9" s="12" customFormat="1">
       <c r="A214" s="11" t="s">
         <v>295</v>
       </c>
@@ -10233,7 +10231,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A215" s="11" t="s">
         <v>297</v>
       </c>
@@ -10258,7 +10256,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A216" s="11" t="s">
         <v>298</v>
       </c>
@@ -10283,7 +10281,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A217" s="11" t="s">
         <v>406</v>
       </c>
@@ -10308,7 +10306,7 @@
       </c>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A218" s="11" t="s">
         <v>407</v>
       </c>
@@ -10333,7 +10331,7 @@
       </c>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A219" s="11" t="s">
         <v>300</v>
       </c>
@@ -10358,7 +10356,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A220" s="11" t="s">
         <v>302</v>
       </c>
@@ -10383,7 +10381,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:9" s="12" customFormat="1">
       <c r="A221" s="11" t="s">
         <v>303</v>
       </c>
@@ -10408,7 +10406,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A222" s="11" t="s">
         <v>305</v>
       </c>
@@ -10433,7 +10431,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:9" s="12" customFormat="1">
       <c r="A223" s="11" t="s">
         <v>308</v>
       </c>
@@ -10458,7 +10456,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A224" s="11" t="s">
         <v>310</v>
       </c>
@@ -10483,7 +10481,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:9" s="12" customFormat="1">
       <c r="A225" s="11" t="s">
         <v>885</v>
       </c>
@@ -10508,7 +10506,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:9" s="12" customFormat="1">
       <c r="A226" s="11" t="s">
         <v>886</v>
       </c>
@@ -10533,7 +10531,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A227" s="11" t="s">
         <v>889</v>
       </c>
@@ -10558,7 +10556,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" s="12" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:9" s="12" customFormat="1" ht="135">
       <c r="A228" s="11" t="s">
         <v>312</v>
       </c>
@@ -10583,7 +10581,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:9" s="12" customFormat="1">
       <c r="A229" s="11" t="s">
         <v>314</v>
       </c>
@@ -10608,7 +10606,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:9" s="12" customFormat="1">
       <c r="A230" s="11" t="s">
         <v>315</v>
       </c>
@@ -10633,7 +10631,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A231" s="11" t="s">
         <v>891</v>
       </c>
@@ -10658,7 +10656,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" s="12" customFormat="1" ht="216" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:9" s="12" customFormat="1" ht="210">
       <c r="A232" s="11" t="s">
         <v>316</v>
       </c>
@@ -10683,7 +10681,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A233" s="11" t="s">
         <v>318</v>
       </c>
@@ -10708,7 +10706,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A234" s="11" t="s">
         <v>319</v>
       </c>
@@ -10733,7 +10731,7 @@
       </c>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A235" s="11" t="s">
         <v>617</v>
       </c>
@@ -10760,7 +10758,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="236" spans="1:9" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A236" s="11" t="s">
         <v>411</v>
       </c>
@@ -10785,7 +10783,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A237" s="11" t="s">
         <v>320</v>
       </c>
@@ -10812,7 +10810,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="238" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:9" s="12" customFormat="1">
       <c r="A238" s="11" t="s">
         <v>469</v>
       </c>
@@ -10837,7 +10835,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:9" s="12" customFormat="1" ht="75">
       <c r="A239" s="11" t="s">
         <v>322</v>
       </c>
@@ -10864,7 +10862,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="240" spans="1:9" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:9" s="12" customFormat="1" ht="45">
       <c r="A240" s="11" t="s">
         <v>326</v>
       </c>
@@ -10889,7 +10887,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:9" s="12" customFormat="1" ht="30">
       <c r="A241" s="11" t="s">
         <v>328</v>
       </c>
@@ -10914,7 +10912,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A242" s="34" t="s">
         <v>670</v>
       </c>
@@ -10943,7 +10941,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="243" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A243" s="34" t="s">
         <v>673</v>
       </c>
@@ -10972,7 +10970,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="244" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A244" s="34" t="s">
         <v>674</v>
       </c>
@@ -11001,7 +10999,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="245" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A245" s="34" t="s">
         <v>583</v>
       </c>
@@ -11030,7 +11028,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="246" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A246" s="34" t="s">
         <v>584</v>
       </c>
@@ -11059,7 +11057,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="247" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A247" s="34" t="s">
         <v>587</v>
       </c>
@@ -11088,7 +11086,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="248" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A248" s="34" t="s">
         <v>211</v>
       </c>
@@ -11117,7 +11115,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="249" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A249" s="34" t="s">
         <v>212</v>
       </c>
@@ -11144,7 +11142,7 @@
       </c>
       <c r="I249" s="35"/>
     </row>
-    <row r="250" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A250" s="34" t="s">
         <v>417</v>
       </c>
@@ -11171,7 +11169,7 @@
       </c>
       <c r="I250" s="35"/>
     </row>
-    <row r="251" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A251" s="34" t="s">
         <v>418</v>
       </c>
@@ -11198,7 +11196,7 @@
       </c>
       <c r="I251" s="35"/>
     </row>
-    <row r="252" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A252" s="34" t="s">
         <v>419</v>
       </c>
@@ -11225,7 +11223,7 @@
       </c>
       <c r="I252" s="35"/>
     </row>
-    <row r="253" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A253" s="34" t="s">
         <v>420</v>
       </c>
@@ -11252,7 +11250,7 @@
       </c>
       <c r="I253" s="35"/>
     </row>
-    <row r="254" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A254" s="34" t="s">
         <v>421</v>
       </c>
@@ -11279,7 +11277,7 @@
       </c>
       <c r="I254" s="35"/>
     </row>
-    <row r="255" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A255" s="34" t="s">
         <v>422</v>
       </c>
@@ -11306,7 +11304,7 @@
       </c>
       <c r="I255" s="35"/>
     </row>
-    <row r="256" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A256" s="34" t="s">
         <v>423</v>
       </c>
@@ -11333,7 +11331,7 @@
       </c>
       <c r="I256" s="35"/>
     </row>
-    <row r="257" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A257" s="34" t="s">
         <v>424</v>
       </c>
@@ -11360,7 +11358,7 @@
       </c>
       <c r="I257" s="35"/>
     </row>
-    <row r="258" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A258" s="34" t="s">
         <v>425</v>
       </c>
@@ -11387,7 +11385,7 @@
       </c>
       <c r="I258" s="35"/>
     </row>
-    <row r="259" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A259" s="34" t="s">
         <v>426</v>
       </c>
@@ -11414,7 +11412,7 @@
       </c>
       <c r="I259" s="35"/>
     </row>
-    <row r="260" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A260" s="34" t="s">
         <v>427</v>
       </c>
@@ -11441,7 +11439,7 @@
       </c>
       <c r="I260" s="35"/>
     </row>
-    <row r="261" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A261" s="34" t="s">
         <v>428</v>
       </c>
@@ -11468,7 +11466,7 @@
       </c>
       <c r="I261" s="35"/>
     </row>
-    <row r="262" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A262" s="34" t="s">
         <v>475</v>
       </c>
@@ -11495,7 +11493,7 @@
       </c>
       <c r="I262" s="35"/>
     </row>
-    <row r="263" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A263" s="34" t="s">
         <v>329</v>
       </c>
@@ -11524,7 +11522,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="264" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A264" s="34" t="s">
         <v>476</v>
       </c>
@@ -11551,7 +11549,7 @@
       </c>
       <c r="I264" s="35"/>
     </row>
-    <row r="265" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A265" s="34" t="s">
         <v>477</v>
       </c>
@@ -11578,7 +11576,7 @@
       </c>
       <c r="I265" s="35"/>
     </row>
-    <row r="266" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A266" s="34" t="s">
         <v>478</v>
       </c>
@@ -11605,7 +11603,7 @@
       </c>
       <c r="I266" s="35"/>
     </row>
-    <row r="267" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A267" s="34" t="s">
         <v>479</v>
       </c>
@@ -11632,7 +11630,7 @@
       </c>
       <c r="I267" s="35"/>
     </row>
-    <row r="268" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A268" s="34" t="s">
         <v>480</v>
       </c>
@@ -11659,7 +11657,7 @@
       </c>
       <c r="I268" s="35"/>
     </row>
-    <row r="269" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A269" s="34" t="s">
         <v>481</v>
       </c>
@@ -11686,7 +11684,7 @@
       </c>
       <c r="I269" s="35"/>
     </row>
-    <row r="270" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A270" s="34" t="s">
         <v>912</v>
       </c>
@@ -11713,7 +11711,7 @@
       </c>
       <c r="I270" s="35"/>
     </row>
-    <row r="271" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A271" s="34" t="s">
         <v>482</v>
       </c>
@@ -11740,7 +11738,7 @@
       </c>
       <c r="I271" s="35"/>
     </row>
-    <row r="272" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A272" s="34" t="s">
         <v>483</v>
       </c>
@@ -11767,7 +11765,7 @@
       </c>
       <c r="I272" s="35"/>
     </row>
-    <row r="273" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A273" s="34" t="s">
         <v>484</v>
       </c>
@@ -11794,7 +11792,7 @@
       </c>
       <c r="I273" s="35"/>
     </row>
-    <row r="274" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A274" s="34" t="s">
         <v>485</v>
       </c>
@@ -11821,7 +11819,7 @@
       </c>
       <c r="I274" s="35"/>
     </row>
-    <row r="275" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A275" s="34" t="s">
         <v>486</v>
       </c>
@@ -11848,7 +11846,7 @@
       </c>
       <c r="I275" s="35"/>
     </row>
-    <row r="276" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A276" s="34" t="s">
         <v>487</v>
       </c>
@@ -11875,7 +11873,7 @@
       </c>
       <c r="I276" s="35"/>
     </row>
-    <row r="277" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A277" s="34" t="s">
         <v>488</v>
       </c>
@@ -11902,7 +11900,7 @@
       </c>
       <c r="I277" s="35"/>
     </row>
-    <row r="278" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A278" s="34" t="s">
         <v>606</v>
       </c>
@@ -11929,7 +11927,7 @@
       </c>
       <c r="I278" s="35"/>
     </row>
-    <row r="279" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A279" s="34" t="s">
         <v>607</v>
       </c>
@@ -11958,7 +11956,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="280" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A280" s="34" t="s">
         <v>608</v>
       </c>
@@ -11987,7 +11985,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="281" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A281" s="34" t="s">
         <v>609</v>
       </c>
@@ -12016,7 +12014,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="282" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A282" s="34" t="s">
         <v>610</v>
       </c>
@@ -12045,7 +12043,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="283" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A283" s="34" t="s">
         <v>611</v>
       </c>
@@ -12074,7 +12072,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="284" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A284" s="34" t="s">
         <v>612</v>
       </c>
@@ -12103,7 +12101,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="285" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A285" s="34" t="s">
         <v>330</v>
       </c>
@@ -12132,7 +12130,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="286" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A286" s="34" t="s">
         <v>578</v>
       </c>
@@ -12161,7 +12159,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="287" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A287" s="34" t="s">
         <v>579</v>
       </c>
@@ -12188,7 +12186,7 @@
       </c>
       <c r="I287" s="37"/>
     </row>
-    <row r="288" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A288" s="34" t="s">
         <v>894</v>
       </c>
@@ -12215,7 +12213,7 @@
       </c>
       <c r="I288" s="35"/>
     </row>
-    <row r="289" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A289" s="34" t="s">
         <v>895</v>
       </c>
@@ -12244,7 +12242,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="290" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A290" s="34" t="s">
         <v>246</v>
       </c>
@@ -12273,7 +12271,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="291" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A291" s="34" t="s">
         <v>433</v>
       </c>
@@ -12300,7 +12298,7 @@
       </c>
       <c r="I291" s="35"/>
     </row>
-    <row r="292" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A292" s="34" t="s">
         <v>434</v>
       </c>
@@ -12327,7 +12325,7 @@
       </c>
       <c r="I292" s="35"/>
     </row>
-    <row r="293" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A293" s="34" t="s">
         <v>435</v>
       </c>
@@ -12354,7 +12352,7 @@
       </c>
       <c r="I293" s="35"/>
     </row>
-    <row r="294" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A294" s="34" t="s">
         <v>436</v>
       </c>
@@ -12381,7 +12379,7 @@
       </c>
       <c r="I294" s="35"/>
     </row>
-    <row r="295" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A295" s="34" t="s">
         <v>437</v>
       </c>
@@ -12408,7 +12406,7 @@
       </c>
       <c r="I295" s="35"/>
     </row>
-    <row r="296" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A296" s="34" t="s">
         <v>438</v>
       </c>
@@ -12435,7 +12433,7 @@
       </c>
       <c r="I296" s="35"/>
     </row>
-    <row r="297" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A297" s="34" t="s">
         <v>439</v>
       </c>
@@ -12462,7 +12460,7 @@
       </c>
       <c r="I297" s="35"/>
     </row>
-    <row r="298" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A298" s="34" t="s">
         <v>440</v>
       </c>
@@ -12489,7 +12487,7 @@
       </c>
       <c r="I298" s="35"/>
     </row>
-    <row r="299" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A299" s="34" t="s">
         <v>441</v>
       </c>
@@ -12516,7 +12514,7 @@
       </c>
       <c r="I299" s="35"/>
     </row>
-    <row r="300" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A300" s="34" t="s">
         <v>442</v>
       </c>
@@ -12543,7 +12541,7 @@
       </c>
       <c r="I300" s="35"/>
     </row>
-    <row r="301" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A301" s="34" t="s">
         <v>443</v>
       </c>
@@ -12570,7 +12568,7 @@
       </c>
       <c r="I301" s="35"/>
     </row>
-    <row r="302" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A302" s="34" t="s">
         <v>575</v>
       </c>
@@ -12597,7 +12595,7 @@
       </c>
       <c r="I302" s="35"/>
     </row>
-    <row r="303" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A303" s="34" t="s">
         <v>444</v>
       </c>
@@ -12624,7 +12622,7 @@
       </c>
       <c r="I303" s="35"/>
     </row>
-    <row r="304" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A304" s="34" t="s">
         <v>445</v>
       </c>
@@ -12651,7 +12649,7 @@
       </c>
       <c r="I304" s="35"/>
     </row>
-    <row r="305" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A305" s="34" t="s">
         <v>513</v>
       </c>
@@ -12678,7 +12676,7 @@
       </c>
       <c r="I305" s="35"/>
     </row>
-    <row r="306" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A306" s="34" t="s">
         <v>526</v>
       </c>
@@ -12707,7 +12705,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="307" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A307" s="34" t="s">
         <v>331</v>
       </c>
@@ -12736,7 +12734,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="308" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A308" s="34" t="s">
         <v>491</v>
       </c>
@@ -12763,7 +12761,7 @@
       </c>
       <c r="I308" s="35"/>
     </row>
-    <row r="309" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A309" s="34" t="s">
         <v>492</v>
       </c>
@@ -12790,7 +12788,7 @@
       </c>
       <c r="I309" s="35"/>
     </row>
-    <row r="310" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A310" s="34" t="s">
         <v>493</v>
       </c>
@@ -12817,7 +12815,7 @@
       </c>
       <c r="I310" s="35"/>
     </row>
-    <row r="311" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A311" s="34" t="s">
         <v>494</v>
       </c>
@@ -12844,7 +12842,7 @@
       </c>
       <c r="I311" s="35"/>
     </row>
-    <row r="312" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A312" s="34" t="s">
         <v>495</v>
       </c>
@@ -12871,7 +12869,7 @@
       </c>
       <c r="I312" s="35"/>
     </row>
-    <row r="313" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A313" s="34" t="s">
         <v>496</v>
       </c>
@@ -12898,7 +12896,7 @@
       </c>
       <c r="I313" s="35"/>
     </row>
-    <row r="314" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A314" s="34" t="s">
         <v>911</v>
       </c>
@@ -12925,7 +12923,7 @@
       </c>
       <c r="I314" s="35"/>
     </row>
-    <row r="315" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A315" s="34" t="s">
         <v>497</v>
       </c>
@@ -12952,7 +12950,7 @@
       </c>
       <c r="I315" s="35"/>
     </row>
-    <row r="316" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A316" s="34" t="s">
         <v>498</v>
       </c>
@@ -12979,7 +12977,7 @@
       </c>
       <c r="I316" s="35"/>
     </row>
-    <row r="317" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A317" s="34" t="s">
         <v>499</v>
       </c>
@@ -13006,7 +13004,7 @@
       </c>
       <c r="I317" s="35"/>
     </row>
-    <row r="318" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A318" s="34" t="s">
         <v>500</v>
       </c>
@@ -13033,7 +13031,7 @@
       </c>
       <c r="I318" s="35"/>
     </row>
-    <row r="319" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A319" s="34" t="s">
         <v>501</v>
       </c>
@@ -13060,7 +13058,7 @@
       </c>
       <c r="I319" s="35"/>
     </row>
-    <row r="320" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A320" s="34" t="s">
         <v>576</v>
       </c>
@@ -13087,7 +13085,7 @@
       </c>
       <c r="I320" s="35"/>
     </row>
-    <row r="321" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A321" s="34" t="s">
         <v>502</v>
       </c>
@@ -13114,7 +13112,7 @@
       </c>
       <c r="I321" s="35"/>
     </row>
-    <row r="322" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A322" s="34" t="s">
         <v>503</v>
       </c>
@@ -13141,7 +13139,7 @@
       </c>
       <c r="I322" s="35"/>
     </row>
-    <row r="323" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A323" s="34" t="s">
         <v>504</v>
       </c>
@@ -13170,7 +13168,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="324" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A324" s="34" t="s">
         <v>332</v>
       </c>
@@ -13199,7 +13197,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="325" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A325" s="34" t="s">
         <v>592</v>
       </c>
@@ -13228,7 +13226,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="326" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A326" s="34" t="s">
         <v>590</v>
       </c>
@@ -13257,7 +13255,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="327" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A327" s="34" t="s">
         <v>591</v>
       </c>
@@ -13286,7 +13284,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="328" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A328" s="34" t="s">
         <v>517</v>
       </c>
@@ -13315,7 +13313,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="329" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A329" s="34" t="s">
         <v>596</v>
       </c>
@@ -13344,7 +13342,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="330" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A330" s="34" t="s">
         <v>597</v>
       </c>
@@ -13373,7 +13371,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="331" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A331" s="34" t="s">
         <v>598</v>
       </c>
@@ -13402,7 +13400,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="332" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A332" s="34" t="s">
         <v>599</v>
       </c>
@@ -13428,7 +13426,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="333" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A333" s="34" t="s">
         <v>541</v>
       </c>
@@ -13457,7 +13455,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="334" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A334" s="34" t="s">
         <v>333</v>
       </c>
@@ -13486,7 +13484,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="335" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A335" s="34" t="s">
         <v>901</v>
       </c>
@@ -13515,7 +13513,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="336" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A336" s="34" t="s">
         <v>914</v>
       </c>
@@ -13542,7 +13540,7 @@
       </c>
       <c r="I336" s="35"/>
     </row>
-    <row r="337" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A337" s="34" t="s">
         <v>902</v>
       </c>
@@ -13571,7 +13569,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="338" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A338" s="34" t="s">
         <v>915</v>
       </c>
@@ -13598,7 +13596,7 @@
       </c>
       <c r="I338" s="35"/>
     </row>
-    <row r="339" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A339" s="34" t="s">
         <v>618</v>
       </c>
@@ -13627,7 +13625,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="340" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A340" s="34" t="s">
         <v>619</v>
       </c>
@@ -13654,7 +13652,7 @@
       </c>
       <c r="I340" s="35"/>
     </row>
-    <row r="341" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A341" s="34" t="s">
         <v>620</v>
       </c>
@@ -13681,7 +13679,7 @@
       </c>
       <c r="I341" s="35"/>
     </row>
-    <row r="342" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A342" s="34" t="s">
         <v>623</v>
       </c>
@@ -13710,7 +13708,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="343" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A343" s="34" t="s">
         <v>624</v>
       </c>
@@ -13737,7 +13735,7 @@
       </c>
       <c r="I343" s="37"/>
     </row>
-    <row r="344" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A344" s="34" t="s">
         <v>625</v>
       </c>
@@ -13764,7 +13762,7 @@
       </c>
       <c r="I344" s="37"/>
     </row>
-    <row r="345" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A345" s="34" t="s">
         <v>321</v>
       </c>
@@ -13793,7 +13791,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="346" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A346" s="34" t="s">
         <v>615</v>
       </c>
@@ -13822,7 +13820,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="347" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A347" s="34" t="s">
         <v>323</v>
       </c>
@@ -13851,7 +13849,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="348" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A348" s="34" t="s">
         <v>324</v>
       </c>
@@ -13878,7 +13876,7 @@
       </c>
       <c r="I348" s="35"/>
     </row>
-    <row r="349" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A349" s="34" t="s">
         <v>448</v>
       </c>
@@ -13905,7 +13903,7 @@
       </c>
       <c r="I349" s="35"/>
     </row>
-    <row r="350" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A350" s="34" t="s">
         <v>449</v>
       </c>
@@ -13932,7 +13930,7 @@
       </c>
       <c r="I350" s="35"/>
     </row>
-    <row r="351" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A351" s="34" t="s">
         <v>450</v>
       </c>
@@ -13959,7 +13957,7 @@
       </c>
       <c r="I351" s="35"/>
     </row>
-    <row r="352" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A352" s="34" t="s">
         <v>451</v>
       </c>
@@ -13986,7 +13984,7 @@
       </c>
       <c r="I352" s="35"/>
     </row>
-    <row r="353" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A353" s="34" t="s">
         <v>452</v>
       </c>
@@ -14013,7 +14011,7 @@
       </c>
       <c r="I353" s="35"/>
     </row>
-    <row r="354" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A354" s="34" t="s">
         <v>453</v>
       </c>
@@ -14040,7 +14038,7 @@
       </c>
       <c r="I354" s="35"/>
     </row>
-    <row r="355" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A355" s="34" t="s">
         <v>454</v>
       </c>
@@ -14067,7 +14065,7 @@
       </c>
       <c r="I355" s="35"/>
     </row>
-    <row r="356" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A356" s="34" t="s">
         <v>455</v>
       </c>
@@ -14094,7 +14092,7 @@
       </c>
       <c r="I356" s="35"/>
     </row>
-    <row r="357" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A357" s="34" t="s">
         <v>456</v>
       </c>
@@ -14121,7 +14119,7 @@
       </c>
       <c r="I357" s="35"/>
     </row>
-    <row r="358" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A358" s="38" t="s">
         <v>631</v>
       </c>
@@ -14148,7 +14146,7 @@
       </c>
       <c r="I358" s="35"/>
     </row>
-    <row r="359" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A359" s="38" t="s">
         <v>632</v>
       </c>
@@ -14175,7 +14173,7 @@
       </c>
       <c r="I359" s="35"/>
     </row>
-    <row r="360" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A360" s="34" t="s">
         <v>457</v>
       </c>
@@ -14202,7 +14200,7 @@
       </c>
       <c r="I360" s="35"/>
     </row>
-    <row r="361" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="361" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A361" s="34" t="s">
         <v>458</v>
       </c>
@@ -14229,7 +14227,7 @@
       </c>
       <c r="I361" s="35"/>
     </row>
-    <row r="362" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A362" s="34" t="s">
         <v>527</v>
       </c>
@@ -14258,7 +14256,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="363" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A363" s="34" t="s">
         <v>325</v>
       </c>
@@ -14285,7 +14283,7 @@
       </c>
       <c r="I363" s="35"/>
     </row>
-    <row r="364" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="364" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A364" s="34" t="s">
         <v>459</v>
       </c>
@@ -14312,7 +14310,7 @@
       </c>
       <c r="I364" s="35"/>
     </row>
-    <row r="365" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="365" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A365" s="34" t="s">
         <v>460</v>
       </c>
@@ -14339,7 +14337,7 @@
       </c>
       <c r="I365" s="35"/>
     </row>
-    <row r="366" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="366" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A366" s="34" t="s">
         <v>461</v>
       </c>
@@ -14366,7 +14364,7 @@
       </c>
       <c r="I366" s="35"/>
     </row>
-    <row r="367" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="367" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A367" s="34" t="s">
         <v>462</v>
       </c>
@@ -14393,7 +14391,7 @@
       </c>
       <c r="I367" s="35"/>
     </row>
-    <row r="368" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="368" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A368" s="34" t="s">
         <v>463</v>
       </c>
@@ -14420,7 +14418,7 @@
       </c>
       <c r="I368" s="35"/>
     </row>
-    <row r="369" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="369" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A369" s="34" t="s">
         <v>464</v>
       </c>
@@ -14447,7 +14445,7 @@
       </c>
       <c r="I369" s="35"/>
     </row>
-    <row r="370" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="370" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A370" s="34" t="s">
         <v>465</v>
       </c>
@@ -14474,7 +14472,7 @@
       </c>
       <c r="I370" s="35"/>
     </row>
-    <row r="371" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="371" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A371" s="34" t="s">
         <v>466</v>
       </c>
@@ -14501,7 +14499,7 @@
       </c>
       <c r="I371" s="35"/>
     </row>
-    <row r="372" spans="1:9" s="36" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="372" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A372" s="34" t="s">
         <v>467</v>
       </c>
@@ -14528,7 +14526,7 @@
       </c>
       <c r="I372" s="35"/>
     </row>
-    <row r="373" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="373" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A373" s="34" t="s">
         <v>468</v>
       </c>
@@ -14555,7 +14553,7 @@
       </c>
       <c r="I373" s="35"/>
     </row>
-    <row r="374" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="374" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A374" s="34" t="s">
         <v>518</v>
       </c>
@@ -14582,7 +14580,7 @@
       </c>
       <c r="I374" s="35"/>
     </row>
-    <row r="375" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="375" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A375" s="34" t="s">
         <v>633</v>
       </c>
@@ -14609,7 +14607,7 @@
       </c>
       <c r="I375" s="35"/>
     </row>
-    <row r="376" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="376" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A376" s="34" t="s">
         <v>334</v>
       </c>
@@ -14636,7 +14634,7 @@
       </c>
       <c r="I376" s="37"/>
     </row>
-    <row r="377" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="377" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A377" s="34" t="s">
         <v>335</v>
       </c>
@@ -14663,7 +14661,7 @@
       </c>
       <c r="I377" s="37"/>
     </row>
-    <row r="378" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="378" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A378" s="34" t="s">
         <v>634</v>
       </c>
@@ -14692,7 +14690,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="379" spans="1:9" s="36" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="379" spans="1:9" s="36" customFormat="1" ht="60">
       <c r="A379" s="34" t="s">
         <v>635</v>
       </c>
@@ -14721,7 +14719,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="380" spans="1:9" s="36" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="380" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A380" s="34" t="s">
         <v>636</v>
       </c>
@@ -14748,7 +14746,7 @@
       </c>
       <c r="I380" s="35"/>
     </row>
-    <row r="381" spans="1:9" s="36" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="381" spans="1:9" s="36" customFormat="1" ht="90">
       <c r="A381" s="34" t="s">
         <v>506</v>
       </c>
@@ -14777,7 +14775,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="382" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="382" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A382" s="34" t="s">
         <v>336</v>
       </c>
@@ -14804,7 +14802,7 @@
       </c>
       <c r="I382" s="35"/>
     </row>
-    <row r="383" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="383" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A383" s="34" t="s">
         <v>637</v>
       </c>
@@ -14831,7 +14829,7 @@
       </c>
       <c r="I383" s="35"/>
     </row>
-    <row r="384" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="384" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A384" s="34" t="s">
         <v>638</v>
       </c>
@@ -14858,7 +14856,7 @@
       </c>
       <c r="I384" s="35"/>
     </row>
-    <row r="385" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="385" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A385" s="34" t="s">
         <v>639</v>
       </c>
@@ -14885,7 +14883,7 @@
       </c>
       <c r="I385" s="35"/>
     </row>
-    <row r="386" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="386" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A386" s="34" t="s">
         <v>640</v>
       </c>
@@ -14912,7 +14910,7 @@
       </c>
       <c r="I386" s="35"/>
     </row>
-    <row r="387" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="387" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A387" s="34" t="s">
         <v>641</v>
       </c>
@@ -14939,7 +14937,7 @@
       </c>
       <c r="I387" s="35"/>
     </row>
-    <row r="388" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="388" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A388" s="34" t="s">
         <v>642</v>
       </c>
@@ -14966,7 +14964,7 @@
       </c>
       <c r="I388" s="35"/>
     </row>
-    <row r="389" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="389" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A389" s="34" t="s">
         <v>643</v>
       </c>
@@ -14993,7 +14991,7 @@
       </c>
       <c r="I389" s="35"/>
     </row>
-    <row r="390" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="390" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A390" s="34" t="s">
         <v>644</v>
       </c>
@@ -15020,7 +15018,7 @@
       </c>
       <c r="I390" s="35"/>
     </row>
-    <row r="391" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="391" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A391" s="34" t="s">
         <v>645</v>
       </c>
@@ -15047,7 +15045,7 @@
       </c>
       <c r="I391" s="35"/>
     </row>
-    <row r="392" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="392" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A392" s="34" t="s">
         <v>646</v>
       </c>
@@ -15074,7 +15072,7 @@
       </c>
       <c r="I392" s="35"/>
     </row>
-    <row r="393" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="393" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A393" s="34" t="s">
         <v>647</v>
       </c>
@@ -15101,7 +15099,7 @@
       </c>
       <c r="I393" s="35"/>
     </row>
-    <row r="394" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="394" spans="1:9" s="36" customFormat="1" ht="90">
       <c r="A394" s="34" t="s">
         <v>648</v>
       </c>
@@ -15128,7 +15126,7 @@
       </c>
       <c r="I394" s="35"/>
     </row>
-    <row r="395" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="395" spans="1:9" s="36" customFormat="1" ht="90">
       <c r="A395" s="34" t="s">
         <v>649</v>
       </c>
@@ -15155,7 +15153,7 @@
       </c>
       <c r="I395" s="35"/>
     </row>
-    <row r="396" spans="1:9" s="36" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="396" spans="1:9" s="36" customFormat="1" ht="90">
       <c r="A396" s="34" t="s">
         <v>337</v>
       </c>
@@ -15184,7 +15182,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="397" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="397" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A397" s="38" t="s">
         <v>650</v>
       </c>
@@ -15211,7 +15209,7 @@
       </c>
       <c r="I397" s="35"/>
     </row>
-    <row r="398" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="398" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A398" s="38" t="s">
         <v>651</v>
       </c>
@@ -15238,7 +15236,7 @@
       </c>
       <c r="I398" s="35"/>
     </row>
-    <row r="399" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="399" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A399" s="38" t="s">
         <v>652</v>
       </c>
@@ -15265,7 +15263,7 @@
       </c>
       <c r="I399" s="35"/>
     </row>
-    <row r="400" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="400" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A400" s="38" t="s">
         <v>653</v>
       </c>
@@ -15292,7 +15290,7 @@
       </c>
       <c r="I400" s="35"/>
     </row>
-    <row r="401" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="401" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A401" s="38" t="s">
         <v>654</v>
       </c>
@@ -15319,7 +15317,7 @@
       </c>
       <c r="I401" s="35"/>
     </row>
-    <row r="402" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="402" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A402" s="38" t="s">
         <v>655</v>
       </c>
@@ -15346,7 +15344,7 @@
       </c>
       <c r="I402" s="35"/>
     </row>
-    <row r="403" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="403" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A403" s="38" t="s">
         <v>656</v>
       </c>
@@ -15373,7 +15371,7 @@
       </c>
       <c r="I403" s="35"/>
     </row>
-    <row r="404" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="404" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A404" s="38" t="s">
         <v>657</v>
       </c>
@@ -15400,7 +15398,7 @@
       </c>
       <c r="I404" s="35"/>
     </row>
-    <row r="405" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="405" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A405" s="38" t="s">
         <v>658</v>
       </c>
@@ -15427,7 +15425,7 @@
       </c>
       <c r="I405" s="35"/>
     </row>
-    <row r="406" spans="1:9" s="36" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="406" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A406" s="38" t="s">
         <v>659</v>
       </c>
@@ -15454,7 +15452,7 @@
       </c>
       <c r="I406" s="35"/>
     </row>
-    <row r="407" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="407" spans="1:9" s="36" customFormat="1" ht="90">
       <c r="A407" s="38" t="s">
         <v>660</v>
       </c>
@@ -15481,7 +15479,7 @@
       </c>
       <c r="I407" s="35"/>
     </row>
-    <row r="408" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="408" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A408" s="38" t="s">
         <v>661</v>
       </c>
@@ -15508,7 +15506,7 @@
       </c>
       <c r="I408" s="35"/>
     </row>
-    <row r="409" spans="1:9" s="36" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="409" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A409" s="38" t="s">
         <v>662</v>
       </c>
@@ -15538,18 +15536,18 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="12">
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="D12:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B17:I17"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="D12:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C397:C409 F328:F332 F201:F241 F307:F325 B347:B375 F263:F289 F334:F395">
@@ -16066,12 +16064,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -16120,6 +16112,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
@@ -16129,20 +16127,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16155,4 +16139,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>